<commit_message>
Added index text on background info and criteria for inclusion.
</commit_message>
<xml_diff>
--- a/federalcoviddollars.xlsx
+++ b/federalcoviddollars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\OneDrive\Documents\PhD Fall 2021 - Spring 2022\Merriman RA\Fiscal Futures FY2022\Fiscal-Future-Topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230B3106-8CF7-42B5-81A6-4FE5324D2B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88A9DD2-52BA-4A21-9B49-BDAFCAF1C7B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21300" yWindow="-11955" windowWidth="8640" windowHeight="4545" xr2:uid="{85440E55-7C44-4F4B-A24B-5EBBF184EC98}"/>
+    <workbookView xWindow="11298" yWindow="7854" windowWidth="17280" windowHeight="8994" xr2:uid="{85440E55-7C44-4F4B-A24B-5EBBF184EC98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="134">
   <si>
     <t>Federal Other</t>
   </si>
@@ -95,346 +95,352 @@
     <t>FY</t>
   </si>
   <si>
+    <t>Dollars Received</t>
+  </si>
+  <si>
+    <t>Recipient</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>ISBE</t>
+  </si>
+  <si>
+    <t>Excluded</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Originally deposited into Disaster Reponse Fund and then mostly transferred to State CURE</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Compare to normal federal funding!</t>
+  </si>
+  <si>
+    <t>Excluded-Local Transfer. Would be for general covid recvery (Com Dev?)</t>
+  </si>
+  <si>
+    <t>Health Provider</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Families First</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>LocalFiscalRecovery</t>
+  </si>
+  <si>
+    <t>State of Illinois</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Recipient Type</t>
+  </si>
+  <si>
+    <t>Level 3</t>
+  </si>
+  <si>
+    <t>Agency</t>
+  </si>
+  <si>
+    <t>Government Program</t>
+  </si>
+  <si>
+    <t>American Rescue Plan</t>
+  </si>
+  <si>
+    <t>Education Provider</t>
+  </si>
+  <si>
+    <t>Education Funding</t>
+  </si>
+  <si>
+    <t>Household</t>
+  </si>
+  <si>
+    <t>Child Tax Credit Expansion</t>
+  </si>
+  <si>
+    <t>State &amp; Local Government</t>
+  </si>
+  <si>
+    <t>Child &amp; Family Services</t>
+  </si>
+  <si>
+    <t>Department of Health and Human Services</t>
+  </si>
+  <si>
+    <t>Temporary Assistance for Needy Families</t>
+  </si>
+  <si>
+    <t>HHS</t>
+  </si>
+  <si>
+    <t>Child Care &amp; Development Block Grant</t>
+  </si>
+  <si>
+    <t>Child Care Stabilization Grant Program</t>
+  </si>
+  <si>
+    <t>Coronavirus State and Local Fiscal Recovery Funds</t>
+  </si>
+  <si>
+    <t>Treasury</t>
+  </si>
+  <si>
+    <t>Department of Transportation</t>
+  </si>
+  <si>
+    <t>Capital Investment Grants Program</t>
+  </si>
+  <si>
+    <t>Federal Transit Administration</t>
+  </si>
+  <si>
+    <t>Nutrition Funding</t>
+  </si>
+  <si>
+    <t>US Department of Agriculture</t>
+  </si>
+  <si>
+    <t>Supplemental Nutrition Assistance Program</t>
+  </si>
+  <si>
+    <t>American Rescue Plan Total</t>
+  </si>
+  <si>
+    <t>CARES Act</t>
+  </si>
+  <si>
+    <t>Grants to Health Providers</t>
+  </si>
+  <si>
+    <t>Provider Relief Fund</t>
+  </si>
+  <si>
+    <t>Community Services Block Grant</t>
+  </si>
+  <si>
+    <t>Coronavirus Relief Fund</t>
+  </si>
+  <si>
+    <t>Election Security Grants</t>
+  </si>
+  <si>
+    <t>State &amp; Local Government;Other</t>
+  </si>
+  <si>
+    <t>Head Start</t>
+  </si>
+  <si>
+    <t>CARES Act Total</t>
+  </si>
+  <si>
+    <t>Medicaid Continuous Coverage Requirement</t>
+  </si>
+  <si>
+    <t>Families First Act Total</t>
+  </si>
+  <si>
+    <t>PPP &amp; Health Care Enhancement Act</t>
+  </si>
+  <si>
+    <t>PPP &amp; Health Care Enhancement Act Total</t>
+  </si>
+  <si>
+    <t>Response &amp; Relief Act</t>
+  </si>
+  <si>
+    <t>State Transportation Infrastructure Grants</t>
+  </si>
+  <si>
+    <t>Response &amp; Relief Act Total</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>TANF</t>
+  </si>
+  <si>
+    <t>Human Services</t>
+  </si>
+  <si>
+    <t>Sum of Other items minus TANF &amp; Transit</t>
+  </si>
+  <si>
+    <t>Healthcare Provider Relief Fund - Considered as Medicaid rev</t>
+  </si>
+  <si>
+    <t>Healthcare</t>
+  </si>
+  <si>
+    <t>Edu</t>
+  </si>
+  <si>
+    <t>Gen. Recovery</t>
+  </si>
+  <si>
+    <t>Fund</t>
+  </si>
+  <si>
+    <t>Education Stabilization Fund</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 569 million normal Education stabilization fund + Governors emergency Education GEER fund 108.5 milloin</t>
+  </si>
+  <si>
+    <t>Other money that went to Illinois but not the "State of Illinois" minus Education 677 million</t>
+  </si>
+  <si>
+    <t>SNAP</t>
+  </si>
+  <si>
+    <t>Child &amp; Fam Serv</t>
+  </si>
+  <si>
+    <t>Child Care &amp; Development Block Grant &amp; Community Services Block Grant</t>
+  </si>
+  <si>
+    <t>Election Security, Airlines</t>
+  </si>
+  <si>
+    <t>Child Care &amp; Development Block Grant, transportation, private schools</t>
+  </si>
+  <si>
+    <t>Local Govs-Excluded</t>
+  </si>
+  <si>
+    <t>Legislation2</t>
+  </si>
+  <si>
+    <t>CRRSA</t>
+  </si>
+  <si>
+    <t>Normal Spending 2019</t>
+  </si>
+  <si>
+    <t>Federal - Other</t>
+  </si>
+  <si>
+    <t>Federal Medicaid Reimbursements</t>
+  </si>
+  <si>
+    <t>Federal Transportation</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>2022-2019</t>
+  </si>
+  <si>
+    <t>FedRevCat</t>
+  </si>
+  <si>
+    <t>Federal-Other</t>
+  </si>
+  <si>
+    <t>Local Transfers-Excluded</t>
+  </si>
+  <si>
+    <t>Federal Medicaid</t>
+  </si>
+  <si>
+    <t>Federal K-12</t>
+  </si>
+  <si>
+    <t>UI Fund</t>
+  </si>
+  <si>
+    <t>Capital</t>
+  </si>
+  <si>
+    <t>FY23</t>
+  </si>
+  <si>
+    <t>Rev Replacement??</t>
+  </si>
+  <si>
+    <t>ProgramsFY22</t>
+  </si>
+  <si>
+    <t>2.7?</t>
+  </si>
+  <si>
+    <t>ProgramsFy23</t>
+  </si>
+  <si>
+    <t>Spent</t>
+  </si>
+  <si>
+    <t>FY Spent</t>
+  </si>
+  <si>
+    <t>Allocated</t>
+  </si>
+  <si>
+    <t>State_Local</t>
+  </si>
+  <si>
+    <t>Local Govs</t>
+  </si>
+  <si>
+    <t>State Departments</t>
+  </si>
+  <si>
+    <t>Broad Category</t>
+  </si>
+  <si>
+    <t>State Government</t>
+  </si>
+  <si>
+    <t>Health Provider Fund</t>
+  </si>
+  <si>
+    <t>Law Total</t>
+  </si>
+  <si>
+    <t>CRSSA</t>
+  </si>
+  <si>
+    <t>Recipient Type Amount</t>
+  </si>
+  <si>
+    <t>Part of ARPA State AND Local funds 14.1 Billion</t>
+  </si>
+  <si>
+    <t>FY20</t>
+  </si>
+  <si>
     <t>FY21</t>
   </si>
   <si>
-    <t>Dollars Received</t>
-  </si>
-  <si>
-    <t>Recipient</t>
-  </si>
-  <si>
-    <t>Illinois</t>
-  </si>
-  <si>
-    <t>ISBE</t>
-  </si>
-  <si>
-    <t>Excluded</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Originally deposited into Disaster Reponse Fund and then mostly transferred to State CURE</t>
-  </si>
-  <si>
-    <t>Purpose</t>
-  </si>
-  <si>
-    <t>Compare to normal federal funding!</t>
-  </si>
-  <si>
-    <t>Excluded-Local Transfer. Would be for general covid recvery (Com Dev?)</t>
-  </si>
-  <si>
-    <t>Health Provider</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Families First</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>LocalFiscalRecovery</t>
-  </si>
-  <si>
-    <t>State of Illinois</t>
-  </si>
-  <si>
-    <t>(blank)</t>
-  </si>
-  <si>
-    <t>Row Labels</t>
-  </si>
-  <si>
-    <t>Recipient Type</t>
-  </si>
-  <si>
-    <t>Level 3</t>
-  </si>
-  <si>
-    <t>Agency</t>
-  </si>
-  <si>
-    <t>Government Program</t>
-  </si>
-  <si>
-    <t>American Rescue Plan</t>
-  </si>
-  <si>
-    <t>Education Provider</t>
-  </si>
-  <si>
-    <t>Education Funding</t>
-  </si>
-  <si>
-    <t>Household</t>
-  </si>
-  <si>
-    <t>Child Tax Credit Expansion</t>
-  </si>
-  <si>
-    <t>State &amp; Local Government</t>
-  </si>
-  <si>
-    <t>Child &amp; Family Services</t>
-  </si>
-  <si>
-    <t>Department of Health and Human Services</t>
-  </si>
-  <si>
-    <t>Temporary Assistance for Needy Families</t>
-  </si>
-  <si>
-    <t>HHS</t>
-  </si>
-  <si>
-    <t>Child Care &amp; Development Block Grant</t>
-  </si>
-  <si>
-    <t>Child Care Stabilization Grant Program</t>
-  </si>
-  <si>
-    <t>Coronavirus State and Local Fiscal Recovery Funds</t>
-  </si>
-  <si>
-    <t>Treasury</t>
-  </si>
-  <si>
-    <t>Department of Transportation</t>
-  </si>
-  <si>
-    <t>Capital Investment Grants Program</t>
-  </si>
-  <si>
-    <t>Federal Transit Administration</t>
-  </si>
-  <si>
-    <t>Nutrition Funding</t>
-  </si>
-  <si>
-    <t>US Department of Agriculture</t>
-  </si>
-  <si>
-    <t>Supplemental Nutrition Assistance Program</t>
-  </si>
-  <si>
-    <t>American Rescue Plan Total</t>
-  </si>
-  <si>
-    <t>CARES Act</t>
-  </si>
-  <si>
-    <t>Grants to Health Providers</t>
-  </si>
-  <si>
-    <t>Provider Relief Fund</t>
-  </si>
-  <si>
-    <t>Community Services Block Grant</t>
-  </si>
-  <si>
-    <t>Coronavirus Relief Fund</t>
-  </si>
-  <si>
-    <t>Election Security Grants</t>
-  </si>
-  <si>
-    <t>State &amp; Local Government;Other</t>
-  </si>
-  <si>
-    <t>Head Start</t>
-  </si>
-  <si>
-    <t>CARES Act Total</t>
-  </si>
-  <si>
-    <t>Medicaid Continuous Coverage Requirement</t>
-  </si>
-  <si>
-    <t>Families First Act Total</t>
-  </si>
-  <si>
-    <t>PPP &amp; Health Care Enhancement Act</t>
-  </si>
-  <si>
-    <t>PPP &amp; Health Care Enhancement Act Total</t>
-  </si>
-  <si>
-    <t>Response &amp; Relief Act</t>
-  </si>
-  <si>
-    <t>State Transportation Infrastructure Grants</t>
-  </si>
-  <si>
-    <t>Response &amp; Relief Act Total</t>
-  </si>
-  <si>
-    <t>Grand Total</t>
-  </si>
-  <si>
-    <t>TANF</t>
-  </si>
-  <si>
-    <t>Human Services</t>
-  </si>
-  <si>
-    <t>Sum of Other items minus TANF &amp; Transit</t>
-  </si>
-  <si>
-    <t>Healthcare Provider Relief Fund - Considered as Medicaid rev</t>
-  </si>
-  <si>
-    <t>Healthcare</t>
-  </si>
-  <si>
-    <t>Edu</t>
-  </si>
-  <si>
-    <t>Gen. Recovery</t>
-  </si>
-  <si>
-    <t>Fund</t>
-  </si>
-  <si>
-    <t>Education Stabilization Fund</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 569 million normal Education stabilization fund + Governors emergency Education GEER fund 108.5 milloin</t>
-  </si>
-  <si>
-    <t>Other money that went to Illinois but not the "State of Illinois" minus Education 677 million</t>
-  </si>
-  <si>
-    <t>Nutrition</t>
-  </si>
-  <si>
-    <t>SNAP</t>
-  </si>
-  <si>
-    <t>Child &amp; Fam Serv</t>
-  </si>
-  <si>
-    <t>Child Care &amp; Development Block Grant &amp; Community Services Block Grant</t>
-  </si>
-  <si>
-    <t>Election Security, Airlines</t>
-  </si>
-  <si>
-    <t>PPP &amp; HealthCare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Response &amp;Relief </t>
-  </si>
-  <si>
-    <t>Child Care &amp; Development Block Grant, transportation, private schools</t>
-  </si>
-  <si>
-    <t>Local Govs-Excluded</t>
-  </si>
-  <si>
-    <t>Legislation2</t>
-  </si>
-  <si>
-    <t>CRRSA</t>
-  </si>
-  <si>
-    <t>Normal Spending 2019</t>
-  </si>
-  <si>
-    <t>Federal - Other</t>
-  </si>
-  <si>
-    <t>Federal Medicaid Reimbursements</t>
-  </si>
-  <si>
-    <t>Federal Transportation</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>2022-2019</t>
-  </si>
-  <si>
-    <t>FedRevCat</t>
-  </si>
-  <si>
-    <t>Federal-Other</t>
-  </si>
-  <si>
-    <t>Local Transfers-Excluded</t>
-  </si>
-  <si>
-    <t>Federal Medicaid</t>
-  </si>
-  <si>
-    <t>Federal K-12</t>
-  </si>
-  <si>
-    <t>UI Fund</t>
-  </si>
-  <si>
-    <t>Capital</t>
-  </si>
-  <si>
-    <t>FY23</t>
-  </si>
-  <si>
-    <t>Rev Replacement??</t>
-  </si>
-  <si>
-    <t>ProgramsFY22</t>
-  </si>
-  <si>
-    <t>2.7?</t>
-  </si>
-  <si>
-    <t>ProgramsFy23</t>
-  </si>
-  <si>
-    <t>Spent</t>
-  </si>
-  <si>
-    <t>FY Spent</t>
-  </si>
-  <si>
-    <t>Allocated</t>
-  </si>
-  <si>
-    <t>State_Local</t>
-  </si>
-  <si>
-    <t>Local Govs</t>
-  </si>
-  <si>
-    <t>State Departments</t>
-  </si>
-  <si>
-    <t>Broad Category</t>
-  </si>
-  <si>
-    <t>State Government</t>
-  </si>
-  <si>
-    <t>Health Provider Fund</t>
-  </si>
-  <si>
-    <t>Law Total</t>
-  </si>
-  <si>
-    <t>CRSSA</t>
-  </si>
-  <si>
-    <t>Recipient Type Amount</t>
-  </si>
-  <si>
-    <t>Part of ARPA State AND Local funds 14.1 Billion</t>
+    <t>FF_Cat2</t>
+  </si>
+  <si>
+    <t>Other Federal Revenue</t>
+  </si>
+  <si>
+    <t>PPP &amp; Health Care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response &amp; Relief </t>
   </si>
 </sst>
 </file>
@@ -579,12 +585,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7307C173-B5A8-415C-816E-E5204417BCF6}" name="Table1" displayName="Table1" ref="A1:P22" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:P22" xr:uid="{7307C173-B5A8-415C-816E-E5204417BCF6}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7307C173-B5A8-415C-816E-E5204417BCF6}" name="Table1" displayName="Table1" ref="A1:Q22" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:Q22" xr:uid="{7307C173-B5A8-415C-816E-E5204417BCF6}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P16">
     <sortCondition ref="A1:A16"/>
   </sortState>
-  <tableColumns count="16">
+  <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{8163EC4D-009A-40FF-9229-6E891FB726B7}" name="Legislation"/>
     <tableColumn id="15" xr3:uid="{1FEBC966-86AC-4D2C-92C2-C1CD0A685BD6}" name="Law Total"/>
     <tableColumn id="16" xr3:uid="{E165A898-E314-4F71-AD05-5E8E48123AA0}" name="Recipient Type Amount" dataDxfId="6"/>
@@ -595,6 +601,7 @@
     <tableColumn id="3" xr3:uid="{A82033BA-F431-4547-894C-F29C06EF1849}" name="Recipient"/>
     <tableColumn id="9" xr3:uid="{FA7BFC94-6DAB-48D1-8E20-602FB4C4821C}" name="Fund"/>
     <tableColumn id="4" xr3:uid="{8B66ADA8-3D64-4999-AF9E-0DCECDB0CFDA}" name="Purpose"/>
+    <tableColumn id="17" xr3:uid="{6127FB03-EB5A-466A-A0C0-F2B24523B085}" name="FF_Cat2"/>
     <tableColumn id="5" xr3:uid="{D7BE3FF4-025D-48AC-85BC-582B164E67AF}" name="FF_Cat"/>
     <tableColumn id="12" xr3:uid="{F4DF1D9B-D6F1-4E5B-9116-A9EC7B0CFC4F}" name="FedRevCat"/>
     <tableColumn id="6" xr3:uid="{B76CE084-47E0-4941-8B7B-58AC5FF2037D}" name="FY"/>
@@ -916,7 +923,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -924,80 +931,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB82A071-B66B-4BBA-B527-9BE9A8C2310F}">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="57" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="87" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="23.796875" customWidth="1"/>
+    <col min="1" max="1" width="9.3984375" customWidth="1"/>
     <col min="2" max="3" width="15.3984375" customWidth="1"/>
     <col min="4" max="4" width="9.8984375" customWidth="1"/>
-    <col min="5" max="5" width="15.69921875" customWidth="1"/>
+    <col min="5" max="5" width="9.296875" customWidth="1"/>
     <col min="7" max="7" width="15.69921875" customWidth="1"/>
-    <col min="10" max="10" width="15.69921875" customWidth="1"/>
-    <col min="11" max="11" width="21.09765625" customWidth="1"/>
-    <col min="12" max="12" width="10.44921875" customWidth="1"/>
-    <col min="13" max="13" width="9.34765625" customWidth="1"/>
-    <col min="14" max="14" width="22.25" customWidth="1"/>
-    <col min="15" max="15" width="17.94921875" customWidth="1"/>
-    <col min="16" max="16" width="14.6484375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.09765625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="50.296875" customWidth="1"/>
-    <col min="19" max="19" width="23.75" customWidth="1"/>
+    <col min="10" max="11" width="15.69921875" customWidth="1"/>
+    <col min="12" max="12" width="21.09765625" customWidth="1"/>
+    <col min="13" max="13" width="10.44921875" customWidth="1"/>
+    <col min="14" max="14" width="9.34765625" customWidth="1"/>
+    <col min="15" max="15" width="15.3984375" customWidth="1"/>
+    <col min="16" max="16" width="17.94921875" customWidth="1"/>
+    <col min="17" max="17" width="14.6484375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.09765625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="50.296875" customWidth="1"/>
+    <col min="20" max="20" width="23.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="M1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>24</v>
+      <c r="O1" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1009,42 +1021,45 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I2" t="s">
         <v>12</v>
       </c>
       <c r="J2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L2" t="s">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
-        <v>108</v>
-      </c>
       <c r="M2" t="s">
+        <v>104</v>
+      </c>
+      <c r="N2" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="3">
+      <c r="O2" s="3">
         <v>8127000000</v>
       </c>
-      <c r="O2" t="s">
-        <v>131</v>
-      </c>
-      <c r="P2" s="3"/>
-      <c r="Q2"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="P2" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q2" s="3"/>
+      <c r="R2"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1056,42 +1071,45 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I3" t="s">
         <v>12</v>
       </c>
       <c r="J3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L3" t="s">
-        <v>109</v>
+        <v>22</v>
       </c>
       <c r="M3" t="s">
+        <v>105</v>
+      </c>
+      <c r="N3" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="3">
+      <c r="O3" s="3">
         <v>5930002892</v>
       </c>
-      <c r="O3" t="s">
-        <v>131</v>
-      </c>
-      <c r="P3" s="3"/>
-      <c r="Q3"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="P3" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q3" s="3"/>
+      <c r="R3"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1103,39 +1121,42 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K4" t="s">
+        <v>131</v>
+      </c>
+      <c r="L4" t="s">
         <v>4</v>
       </c>
-      <c r="L4" t="s">
-        <v>108</v>
-      </c>
       <c r="M4" t="s">
+        <v>104</v>
+      </c>
+      <c r="N4" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="3">
+      <c r="O4" s="3">
         <v>5054988054</v>
       </c>
-      <c r="P4" s="3"/>
-      <c r="Q4"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q4" s="3"/>
+      <c r="R4"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1147,39 +1168,42 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J5" t="s">
         <v>8</v>
       </c>
       <c r="K5" t="s">
+        <v>100</v>
+      </c>
+      <c r="L5" t="s">
         <v>8</v>
       </c>
-      <c r="L5" t="s">
-        <v>108</v>
-      </c>
       <c r="M5" t="s">
+        <v>104</v>
+      </c>
+      <c r="N5" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="3">
+      <c r="O5" s="3">
         <v>1615071673</v>
       </c>
-      <c r="O5" t="s">
-        <v>27</v>
-      </c>
-      <c r="P5" s="3"/>
-      <c r="Q5"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="P5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q5" s="3"/>
+      <c r="R5"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1191,39 +1215,42 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K6" t="s">
-        <v>5</v>
+        <v>131</v>
       </c>
       <c r="L6" t="s">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="M6" t="s">
+        <v>104</v>
+      </c>
+      <c r="N6" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="3">
+      <c r="O6" s="3">
         <v>3462363000</v>
       </c>
-      <c r="O6" t="s">
-        <v>27</v>
-      </c>
-      <c r="P6" s="3"/>
-      <c r="Q6"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="P6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" s="3"/>
+      <c r="R6"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1235,39 +1262,42 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K7" t="s">
+        <v>131</v>
+      </c>
+      <c r="L7" t="s">
         <v>0</v>
       </c>
-      <c r="L7" t="s">
-        <v>108</v>
-      </c>
       <c r="M7" t="s">
+        <v>104</v>
+      </c>
+      <c r="N7" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="3">
+      <c r="O7" s="3">
         <v>1440804846</v>
       </c>
-      <c r="O7" t="s">
-        <v>81</v>
-      </c>
-      <c r="P7" s="3"/>
-      <c r="Q7"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="P7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q7" s="3"/>
+      <c r="R7"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1279,39 +1309,42 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K8" t="s">
+        <v>131</v>
+      </c>
+      <c r="L8" t="s">
         <v>1</v>
       </c>
-      <c r="L8" t="s">
-        <v>108</v>
-      </c>
       <c r="M8" t="s">
-        <v>18</v>
-      </c>
-      <c r="N8" s="3">
+        <v>104</v>
+      </c>
+      <c r="N8" t="s">
+        <v>128</v>
+      </c>
+      <c r="O8" s="3">
         <v>3518945000</v>
       </c>
-      <c r="O8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P8" s="3"/>
-      <c r="Q8"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="P8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q8" s="3"/>
+      <c r="R8"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1323,36 +1356,39 @@
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="J9" t="s">
         <v>8</v>
       </c>
       <c r="K9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L9" t="s">
-        <v>109</v>
+        <v>22</v>
       </c>
       <c r="M9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N9" s="3">
+        <v>105</v>
+      </c>
+      <c r="N9" t="s">
+        <v>128</v>
+      </c>
+      <c r="O9" s="3">
         <v>1560856347</v>
       </c>
-      <c r="P9" s="3"/>
-      <c r="Q9"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q9" s="3"/>
+      <c r="R9"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1364,39 +1400,42 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="F10" t="s">
         <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="J10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L10" t="s">
-        <v>109</v>
+        <v>22</v>
       </c>
       <c r="M10" t="s">
-        <v>18</v>
-      </c>
-      <c r="N10" s="3">
+        <v>105</v>
+      </c>
+      <c r="N10" t="s">
+        <v>128</v>
+      </c>
+      <c r="O10" s="3">
         <v>1394688072</v>
       </c>
-      <c r="O10" t="s">
-        <v>28</v>
-      </c>
-      <c r="P10" s="3"/>
-      <c r="Q10"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="P10" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q10" s="3"/>
+      <c r="R10"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1408,42 +1447,45 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I11" t="s">
+        <v>86</v>
+      </c>
+      <c r="J11" t="s">
+        <v>83</v>
+      </c>
+      <c r="K11" t="s">
+        <v>131</v>
+      </c>
+      <c r="L11" t="s">
+        <v>4</v>
+      </c>
+      <c r="M11" t="s">
+        <v>107</v>
+      </c>
+      <c r="N11" t="s">
+        <v>128</v>
+      </c>
+      <c r="O11" s="3">
+        <v>677964975</v>
+      </c>
+      <c r="P11" t="s">
         <v>87</v>
       </c>
-      <c r="J11" t="s">
-        <v>84</v>
-      </c>
-      <c r="K11" t="s">
-        <v>4</v>
-      </c>
-      <c r="L11" t="s">
-        <v>111</v>
-      </c>
-      <c r="M11" t="s">
-        <v>18</v>
-      </c>
-      <c r="N11" s="3">
-        <v>677964975</v>
-      </c>
-      <c r="O11" t="s">
-        <v>88</v>
-      </c>
-      <c r="P11" s="3"/>
-      <c r="Q11"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q11" s="3"/>
+      <c r="R11"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1455,39 +1497,42 @@
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G12" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="H12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K12" t="s">
+        <v>131</v>
+      </c>
+      <c r="L12" t="s">
         <v>0</v>
       </c>
-      <c r="L12" t="s">
-        <v>108</v>
-      </c>
       <c r="M12" t="s">
-        <v>18</v>
-      </c>
-      <c r="N12" s="3">
+        <v>104</v>
+      </c>
+      <c r="N12" t="s">
+        <v>128</v>
+      </c>
+      <c r="O12" s="3">
         <v>695541441</v>
       </c>
-      <c r="P12" s="3"/>
-      <c r="Q12"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q12" s="3"/>
+      <c r="R12"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1499,39 +1544,42 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G13" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K13" t="s">
+        <v>131</v>
+      </c>
+      <c r="L13" t="s">
         <v>0</v>
       </c>
-      <c r="L13" t="s">
-        <v>108</v>
-      </c>
       <c r="M13" t="s">
-        <v>18</v>
-      </c>
-      <c r="N13" s="3">
+        <v>104</v>
+      </c>
+      <c r="N13" t="s">
+        <v>128</v>
+      </c>
+      <c r="O13" s="3">
         <v>165000000</v>
       </c>
-      <c r="P13" s="3"/>
-      <c r="Q13"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q13" s="3"/>
+      <c r="R13"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1543,42 +1591,45 @@
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G14" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I14" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="J14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K14" t="s">
+        <v>106</v>
+      </c>
+      <c r="L14" t="s">
         <v>5</v>
       </c>
-      <c r="L14" t="s">
-        <v>110</v>
-      </c>
       <c r="M14" t="s">
-        <v>18</v>
-      </c>
-      <c r="N14" s="3">
+        <v>106</v>
+      </c>
+      <c r="N14" t="s">
+        <v>128</v>
+      </c>
+      <c r="O14" s="3">
         <v>2636263219</v>
       </c>
-      <c r="O14" t="s">
-        <v>82</v>
-      </c>
-      <c r="P14" s="3"/>
-      <c r="Q14"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="P14" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q14" s="3"/>
+      <c r="R14"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1590,39 +1641,45 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" t="s">
         <v>10</v>
       </c>
       <c r="G15" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H15" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="I15" t="s">
+        <v>29</v>
       </c>
       <c r="J15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K15" t="s">
-        <v>30</v>
+        <v>131</v>
       </c>
       <c r="L15" t="s">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="M15" t="s">
-        <v>18</v>
-      </c>
-      <c r="N15" s="3">
+        <v>104</v>
+      </c>
+      <c r="N15" t="s">
+        <v>128</v>
+      </c>
+      <c r="O15" s="3">
         <v>4984990736</v>
       </c>
-      <c r="O15" t="s">
-        <v>89</v>
-      </c>
-      <c r="P15" s="3"/>
-      <c r="Q15"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="P15" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q15" s="3"/>
+      <c r="R15"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1634,287 +1691,305 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" t="s">
+        <v>122</v>
+      </c>
+      <c r="H16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" t="s">
+        <v>92</v>
+      </c>
+      <c r="J16" t="s">
+        <v>29</v>
+      </c>
+      <c r="K16" t="s">
+        <v>131</v>
+      </c>
+      <c r="L16" t="s">
+        <v>0</v>
+      </c>
+      <c r="M16" t="s">
+        <v>104</v>
+      </c>
+      <c r="N16" t="s">
+        <v>128</v>
+      </c>
+      <c r="O16" s="3">
+        <v>71000000</v>
+      </c>
+      <c r="Q16" s="3"/>
+      <c r="R16"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
         <v>30</v>
-      </c>
-      <c r="G16" t="s">
-        <v>126</v>
-      </c>
-      <c r="H16" t="s">
-        <v>30</v>
-      </c>
-      <c r="I16" t="s">
-        <v>94</v>
-      </c>
-      <c r="J16" t="s">
-        <v>30</v>
-      </c>
-      <c r="K16" t="s">
-        <v>0</v>
-      </c>
-      <c r="L16" t="s">
-        <v>108</v>
-      </c>
-      <c r="M16" t="s">
-        <v>18</v>
-      </c>
-      <c r="N16" s="3">
-        <v>71000000</v>
-      </c>
-      <c r="P16" s="3"/>
-      <c r="Q16"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>31</v>
       </c>
       <c r="B17" s="3">
         <v>4469242245</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" t="s">
+        <v>120</v>
+      </c>
+      <c r="H17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K17" t="s">
+        <v>106</v>
+      </c>
+      <c r="L17" t="s">
+        <v>5</v>
+      </c>
+      <c r="M17" t="s">
+        <v>106</v>
+      </c>
+      <c r="N17" t="s">
+        <v>129</v>
+      </c>
+      <c r="O17" s="4">
+        <v>2440888026</v>
+      </c>
+      <c r="P17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q17" s="3"/>
+      <c r="R17"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
         <v>30</v>
-      </c>
-      <c r="E17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" t="s">
-        <v>124</v>
-      </c>
-      <c r="H17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="K17" t="s">
-        <v>5</v>
-      </c>
-      <c r="L17" t="s">
-        <v>110</v>
-      </c>
-      <c r="M17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N17" s="4">
-        <v>2440888026</v>
-      </c>
-      <c r="O17" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="P17" s="3"/>
-      <c r="Q17"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>31</v>
       </c>
       <c r="B18" s="3">
         <v>4469242245</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G18" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>6</v>
       </c>
       <c r="K18" t="s">
+        <v>106</v>
+      </c>
+      <c r="L18" t="s">
         <v>5</v>
       </c>
-      <c r="L18" t="s">
-        <v>110</v>
-      </c>
       <c r="M18" t="s">
-        <v>18</v>
-      </c>
-      <c r="N18" s="4">
+        <v>106</v>
+      </c>
+      <c r="N18" t="s">
+        <v>129</v>
+      </c>
+      <c r="O18" s="4">
         <v>2028354219</v>
       </c>
-      <c r="O18" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="P18" s="3"/>
-      <c r="Q18"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="P18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q18" s="3"/>
+      <c r="R18"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>132</v>
       </c>
       <c r="B19" s="7">
         <v>2778017202</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G19" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K19" t="s">
+        <v>131</v>
+      </c>
+      <c r="L19" t="s">
         <v>5</v>
       </c>
-      <c r="L19" t="s">
-        <v>110</v>
-      </c>
       <c r="M19" t="s">
-        <v>18</v>
-      </c>
-      <c r="N19" s="4">
+        <v>106</v>
+      </c>
+      <c r="N19" t="s">
+        <v>129</v>
+      </c>
+      <c r="O19" s="4">
         <v>2778017202</v>
       </c>
-      <c r="P19" s="3"/>
-      <c r="Q19"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q19" s="3"/>
+      <c r="R19"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="B20" s="7">
-        <v>3519539632</v>
+        <v>3426118654</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F20" t="s">
         <v>11</v>
       </c>
       <c r="G20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K20" t="s">
+        <v>131</v>
+      </c>
+      <c r="L20" t="s">
         <v>4</v>
       </c>
-      <c r="L20" t="s">
-        <v>111</v>
-      </c>
       <c r="M20" t="s">
-        <v>18</v>
-      </c>
-      <c r="N20" s="3">
+        <v>107</v>
+      </c>
+      <c r="N20" t="s">
+        <v>13</v>
+      </c>
+      <c r="O20" s="3">
         <v>2298709129</v>
       </c>
-      <c r="O20" t="s">
-        <v>27</v>
-      </c>
-      <c r="P20" s="3">
+      <c r="P20" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q20" s="3">
         <v>1679195166.0999999</v>
       </c>
-      <c r="Q20"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R20"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="B21" s="7">
-        <v>3519539632</v>
+        <v>3426118654</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G21" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I21" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K21" t="s">
+        <v>131</v>
+      </c>
+      <c r="L21" t="s">
         <v>0</v>
       </c>
-      <c r="L21" t="s">
-        <v>108</v>
-      </c>
       <c r="M21" t="s">
-        <v>18</v>
-      </c>
-      <c r="N21" s="3">
+        <v>104</v>
+      </c>
+      <c r="N21" t="s">
+        <v>13</v>
+      </c>
+      <c r="O21" s="3">
         <v>771926678</v>
       </c>
-      <c r="P21" s="3">
+      <c r="Q21" s="3">
         <v>150000000</v>
       </c>
-      <c r="Q21"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="R21"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="B22" s="7">
-        <v>3519539632</v>
+        <v>3426118654</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G22" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I22" t="s">
         <v>8</v>
@@ -1923,18 +1998,21 @@
         <v>8</v>
       </c>
       <c r="K22" t="s">
+        <v>100</v>
+      </c>
+      <c r="L22" t="s">
         <v>8</v>
       </c>
-      <c r="L22" t="s">
-        <v>108</v>
-      </c>
       <c r="M22" t="s">
+        <v>104</v>
+      </c>
+      <c r="N22" t="s">
         <v>13</v>
       </c>
-      <c r="N22" s="7">
+      <c r="O22" s="7">
         <v>355482847</v>
       </c>
-      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1962,7 +2040,7 @@
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D2">
         <v>2019</v>
@@ -1977,12 +2055,12 @@
         <v>2022</v>
       </c>
       <c r="I2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D3" s="3">
         <v>5942081608.6500006</v>
@@ -2003,7 +2081,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D4" s="3">
         <v>12066820196.85</v>
@@ -2024,7 +2102,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D5" s="3">
         <v>1362675926.1899998</v>
@@ -2045,7 +2123,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2076,7 +2154,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView zoomScale="57" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
@@ -2094,48 +2172,48 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
-        <v>40</v>
-      </c>
       <c r="F1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
         <v>46</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>47</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>48</v>
-      </c>
-      <c r="E2" t="s">
-        <v>49</v>
       </c>
       <c r="I2" s="3">
         <v>20439923</v>
@@ -2143,19 +2221,19 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" t="s">
         <v>55</v>
-      </c>
-      <c r="E3" t="s">
-        <v>56</v>
       </c>
       <c r="I3" s="3">
         <v>30650898</v>
@@ -2163,19 +2241,19 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I4" s="3">
         <v>1584420775</v>
@@ -2183,19 +2261,19 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" s="3">
         <v>1560856347</v>
@@ -2206,19 +2284,19 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
         <v>75</v>
       </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>76</v>
-      </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I6" s="3">
         <v>355482847</v>
@@ -2226,19 +2304,19 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
         <v>46</v>
       </c>
-      <c r="C7" t="s">
-        <v>47</v>
-      </c>
       <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
         <v>50</v>
-      </c>
-      <c r="E7" t="s">
-        <v>51</v>
       </c>
       <c r="I7" s="3">
         <v>496853094</v>
@@ -2246,19 +2324,19 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
         <v>46</v>
       </c>
-      <c r="C8" t="s">
-        <v>47</v>
-      </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I8" s="3">
         <v>796272357</v>
@@ -2266,19 +2344,19 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
         <v>62</v>
       </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
         <v>63</v>
-      </c>
-      <c r="D9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" t="s">
-        <v>64</v>
       </c>
       <c r="I9" s="3">
         <v>2636263219</v>
@@ -2286,19 +2364,19 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
         <v>46</v>
       </c>
-      <c r="C10" t="s">
-        <v>47</v>
-      </c>
       <c r="D10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" t="s">
         <v>50</v>
-      </c>
-      <c r="E10" t="s">
-        <v>51</v>
       </c>
       <c r="I10" s="3">
         <v>118420119</v>
@@ -2306,19 +2384,19 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
         <v>46</v>
       </c>
-      <c r="C11" t="s">
-        <v>47</v>
-      </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I11" s="3">
         <v>47232781</v>
@@ -2326,19 +2404,19 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s">
         <v>68</v>
-      </c>
-      <c r="C12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" t="s">
-        <v>69</v>
       </c>
       <c r="I12" s="3">
         <v>25855403</v>
@@ -2349,13 +2427,13 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
@@ -2369,13 +2447,13 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
@@ -2386,19 +2464,19 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
         <v>63</v>
-      </c>
-      <c r="D15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" t="s">
-        <v>64</v>
       </c>
       <c r="I15" s="3">
         <v>2778017202</v>
@@ -2406,19 +2484,19 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
         <v>46</v>
       </c>
-      <c r="C16" t="s">
-        <v>47</v>
-      </c>
       <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
         <v>50</v>
-      </c>
-      <c r="E16" t="s">
-        <v>51</v>
       </c>
       <c r="I16" s="3">
         <v>331954027</v>
@@ -2426,19 +2504,19 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
         <v>53</v>
       </c>
-      <c r="D17" t="s">
-        <v>54</v>
-      </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F17" s="3">
         <v>5930002892</v>
@@ -2449,19 +2527,19 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F18" s="3">
         <v>1394688072</v>
@@ -2475,19 +2553,19 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" t="s">
         <v>58</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>59</v>
-      </c>
-      <c r="E19" t="s">
-        <v>60</v>
       </c>
       <c r="I19" s="3">
         <v>13342228.25</v>
@@ -2495,19 +2573,19 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
         <v>58</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>59</v>
-      </c>
-      <c r="E20" t="s">
-        <v>60</v>
       </c>
       <c r="I20" s="3">
         <v>695541441</v>
@@ -2515,13 +2593,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
         <v>41</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>42</v>
-      </c>
-      <c r="C21" t="s">
-        <v>43</v>
       </c>
       <c r="I21" s="3">
         <v>83246346</v>
@@ -2529,13 +2607,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
         <v>44</v>
-      </c>
-      <c r="C22" t="s">
-        <v>45</v>
       </c>
       <c r="I22" s="3">
         <v>3462363000</v>
@@ -2543,13 +2621,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G23" s="3">
         <v>5058601934</v>
@@ -2557,7 +2635,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F24" s="3">
         <v>5930002892</v>
@@ -2574,13 +2652,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G26" s="3">
         <v>677964975</v>
@@ -2588,13 +2666,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G27" s="3">
         <v>13899434</v>
@@ -2602,7 +2680,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F28" s="3">
         <v>2955544419</v>
@@ -2619,7 +2697,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G30" s="3">
         <v>4469242245</v>
@@ -2627,7 +2705,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I32" s="3">
         <v>2778017202</v>
@@ -2635,13 +2713,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" t="s">
         <v>42</v>
-      </c>
-      <c r="C34" t="s">
-        <v>43</v>
       </c>
       <c r="I34" s="3">
         <v>84489804</v>
@@ -2649,13 +2727,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G35" s="3">
         <v>2298709129</v>
@@ -2663,7 +2741,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G36" s="3">
         <v>2298709129</v>
@@ -2674,7 +2752,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F38" s="3">
         <v>8885547311</v>
@@ -2709,13 +2787,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2726,7 +2804,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D2">
         <v>2.7</v>
@@ -2746,13 +2824,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2766,13 +2844,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D4">
         <v>1.5</v>
       </c>
       <c r="E4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2783,13 +2861,13 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D5">
         <v>1.82</v>
       </c>
       <c r="E5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2800,7 +2878,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D6">
         <v>1.3660000000000001</v>

</xml_diff>

<commit_message>
top navigation bar changes in yaml. Figures update in Fedrevreceived
</commit_message>
<xml_diff>
--- a/federalcoviddollars.xlsx
+++ b/federalcoviddollars.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\OneDrive\Documents\PhD Fall 2021 - Spring 2022\Merriman RA\Fiscal Futures FY2022\Fiscal-Future-Topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4886185A-359A-4D65-82F9-399865181A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9965ADB0-BC52-48F3-85A9-B2523D0B10E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{85440E55-7C44-4F4B-A24B-5EBBF184EC98}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{85440E55-7C44-4F4B-A24B-5EBBF184EC98}"/>
   </bookViews>
   <sheets>
     <sheet name="committed dollars" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="136">
   <si>
     <t>Federal Other</t>
   </si>
@@ -444,6 +444,9 @@
   </si>
   <si>
     <t>All went to local governments except for 57 million. In 2019, fed transportation received $1.4 billion. Compare to normal federal funding!</t>
+  </si>
+  <si>
+    <t>Law_order</t>
   </si>
 </sst>
 </file>
@@ -588,12 +591,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7307C173-B5A8-415C-816E-E5204417BCF6}" name="Table1" displayName="Table1" ref="A1:Q23" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:Q23" xr:uid="{7307C173-B5A8-415C-816E-E5204417BCF6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7307C173-B5A8-415C-816E-E5204417BCF6}" name="Table1" displayName="Table1" ref="A1:R23" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:R23" xr:uid="{7307C173-B5A8-415C-816E-E5204417BCF6}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q23">
     <sortCondition ref="L1:L23"/>
   </sortState>
-  <tableColumns count="17">
+  <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{8163EC4D-009A-40FF-9229-6E891FB726B7}" name="Legislation"/>
     <tableColumn id="15" xr3:uid="{1FEBC966-86AC-4D2C-92C2-C1CD0A685BD6}" name="Law Total"/>
     <tableColumn id="16" xr3:uid="{E165A898-E314-4F71-AD05-5E8E48123AA0}" name="Recipient Type Amount" dataDxfId="6"/>
@@ -611,6 +614,7 @@
     <tableColumn id="7" xr3:uid="{B2A84F10-914D-4196-9116-2F0B9D5038FE}" name="Dollars Received" dataDxfId="5" dataCellStyle="Comma"/>
     <tableColumn id="8" xr3:uid="{DA7979E1-12D0-4C64-A6DD-57A1C322A8C6}" name="Notes"/>
     <tableColumn id="11" xr3:uid="{C20D0B62-0410-4DA4-B530-7806C0D21673}" name="Normal Spending 2019" dataDxfId="4" dataCellStyle="Comma"/>
+    <tableColumn id="18" xr3:uid="{75738D65-C45E-4232-9108-D965D5ECB719}" name="Law_order"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -936,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB82A071-B66B-4BBA-B527-9BE9A8C2310F}">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView zoomScale="87" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
@@ -1012,6 +1016,9 @@
       <c r="Q1" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
@@ -1061,24 +1068,26 @@
         <v>119</v>
       </c>
       <c r="Q2" s="3"/>
-      <c r="R2"/>
+      <c r="R2">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="7">
-        <v>15943589463</v>
+        <v>24386112042.25</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
         <v>113</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
         <v>113</v>
@@ -1086,6 +1095,9 @@
       <c r="H3" t="s">
         <v>91</v>
       </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
       <c r="J3" t="s">
         <v>8</v>
       </c>
@@ -1099,13 +1111,18 @@
         <v>101</v>
       </c>
       <c r="N3" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="O3" s="3">
-        <v>1560856347</v>
+        <v>1615071673</v>
+      </c>
+      <c r="P3" t="s">
+        <v>134</v>
       </c>
       <c r="Q3" s="3"/>
-      <c r="R3"/>
+      <c r="R3">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
@@ -1122,7 +1139,7 @@
         <v>113</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
         <v>113</v>
@@ -1131,7 +1148,7 @@
         <v>91</v>
       </c>
       <c r="J4" t="s">
-        <v>81</v>
+        <v>8</v>
       </c>
       <c r="K4" t="s">
         <v>22</v>
@@ -1146,63 +1163,61 @@
         <v>120</v>
       </c>
       <c r="O4" s="3">
-        <v>1394688072</v>
-      </c>
-      <c r="P4" t="s">
-        <v>27</v>
+        <v>1560856347</v>
       </c>
       <c r="Q4" s="3"/>
-      <c r="R4"/>
+      <c r="R4">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="7">
-        <v>24386112042.25</v>
+        <v>15943589463</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>113</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H5" t="s">
-        <v>78</v>
-      </c>
-      <c r="I5" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
       <c r="J5" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K5" t="s">
-        <v>123</v>
+        <v>22</v>
       </c>
       <c r="L5" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="M5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N5" t="s">
-        <v>13</v>
+        <v>120</v>
       </c>
       <c r="O5" s="3">
-        <v>3462363000</v>
+        <v>1394688072</v>
       </c>
       <c r="P5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q5" s="3"/>
-      <c r="R5"/>
+      <c r="R5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
@@ -1219,19 +1234,19 @@
         <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="G6" t="s">
         <v>114</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="I6" t="s">
         <v>29</v>
       </c>
       <c r="J6" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="K6" t="s">
         <v>123</v>
@@ -1246,30 +1261,32 @@
         <v>13</v>
       </c>
       <c r="O6" s="3">
-        <v>1440804846</v>
+        <v>3462363000</v>
       </c>
       <c r="P6" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
       <c r="Q6" s="3"/>
-      <c r="R6"/>
+      <c r="R6">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="7">
-        <v>15943589463</v>
+        <v>24386112042.25</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
         <v>30</v>
       </c>
       <c r="F7" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
         <v>114</v>
@@ -1278,10 +1295,10 @@
         <v>30</v>
       </c>
       <c r="I7" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="J7" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="K7" t="s">
         <v>123</v>
@@ -1293,13 +1310,18 @@
         <v>100</v>
       </c>
       <c r="N7" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="O7" s="3">
-        <v>695541441</v>
+        <v>1440804846</v>
+      </c>
+      <c r="P7" t="s">
+        <v>79</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7"/>
+      <c r="R7">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
@@ -1316,19 +1338,19 @@
         <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G8" t="s">
         <v>114</v>
       </c>
       <c r="H8" t="s">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="I8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K8" t="s">
         <v>123</v>
@@ -1343,39 +1365,41 @@
         <v>120</v>
       </c>
       <c r="O8" s="3">
-        <v>165000000</v>
+        <v>695541441</v>
       </c>
       <c r="Q8" s="3"/>
-      <c r="R8"/>
+      <c r="R8">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>3</v>
       </c>
       <c r="B9" s="7">
-        <v>2778017202</v>
+        <v>15943589463</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="E9" t="s">
         <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="G9" t="s">
         <v>114</v>
       </c>
       <c r="H9" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="I9" t="s">
-        <v>127</v>
+        <v>88</v>
       </c>
       <c r="J9" t="s">
-        <v>127</v>
+        <v>87</v>
       </c>
       <c r="K9" t="s">
         <v>123</v>
@@ -1387,27 +1411,26 @@
         <v>100</v>
       </c>
       <c r="N9" t="s">
-        <v>121</v>
-      </c>
-      <c r="O9" s="4">
-        <v>504000000</v>
-      </c>
-      <c r="P9" t="s">
-        <v>128</v>
+        <v>120</v>
+      </c>
+      <c r="O9" s="3">
+        <v>165000000</v>
       </c>
       <c r="Q9" s="3"/>
-      <c r="R9"/>
+      <c r="R9">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>3</v>
       </c>
       <c r="B10" s="7">
-        <v>3426118654</v>
+        <v>15943589463</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" t="s">
-        <v>93</v>
+        <v>3</v>
       </c>
       <c r="E10" t="s">
         <v>30</v>
@@ -1416,13 +1439,13 @@
         <v>29</v>
       </c>
       <c r="G10" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H10" t="s">
         <v>29</v>
       </c>
       <c r="I10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J10" t="s">
         <v>29</v>
@@ -1437,26 +1460,26 @@
         <v>100</v>
       </c>
       <c r="N10" t="s">
-        <v>13</v>
+        <v>120</v>
       </c>
       <c r="O10" s="3">
-        <v>771926678</v>
-      </c>
-      <c r="Q10" s="3">
-        <v>150000000</v>
-      </c>
-      <c r="R10"/>
+        <v>71000000</v>
+      </c>
+      <c r="Q10" s="3"/>
+      <c r="R10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>93</v>
       </c>
       <c r="B11" s="7">
-        <v>15943589463</v>
+        <v>3426118654</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>93</v>
       </c>
       <c r="E11" t="s">
         <v>30</v>
@@ -1465,13 +1488,13 @@
         <v>29</v>
       </c>
       <c r="G11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H11" t="s">
         <v>29</v>
       </c>
       <c r="I11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J11" t="s">
         <v>29</v>
@@ -1486,71 +1509,80 @@
         <v>100</v>
       </c>
       <c r="N11" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="O11" s="3">
-        <v>71000000</v>
-      </c>
-      <c r="Q11" s="3"/>
-      <c r="R11"/>
+        <v>771926678</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>150000000</v>
+      </c>
+      <c r="R11">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>125</v>
       </c>
       <c r="B12" s="7">
-        <v>24386112042.25</v>
+        <v>2778017202</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
         <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="G12" t="s">
         <v>114</v>
       </c>
       <c r="H12" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="I12" t="s">
-        <v>83</v>
+        <v>127</v>
       </c>
       <c r="J12" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
       <c r="K12" t="s">
         <v>123</v>
       </c>
       <c r="L12" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M12" t="s">
         <v>100</v>
       </c>
       <c r="N12" t="s">
-        <v>13</v>
-      </c>
-      <c r="O12" s="3">
-        <v>5054988054</v>
+        <v>121</v>
+      </c>
+      <c r="O12" s="4">
+        <v>504000000</v>
+      </c>
+      <c r="P12" t="s">
+        <v>128</v>
       </c>
       <c r="Q12" s="3"/>
-      <c r="R12"/>
+      <c r="R12">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" s="7">
-        <v>15943589463</v>
+        <v>24386112042.25</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13" t="s">
         <v>30</v>
@@ -1580,27 +1612,26 @@
         <v>100</v>
       </c>
       <c r="N13" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="O13" s="3">
-        <v>677964975</v>
-      </c>
-      <c r="P13" t="s">
-        <v>84</v>
+        <v>5054988054</v>
       </c>
       <c r="Q13" s="3"/>
-      <c r="R13"/>
+      <c r="R13">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>3</v>
       </c>
       <c r="B14" s="7">
-        <v>3426118654</v>
+        <v>15943589463</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" t="s">
-        <v>93</v>
+        <v>3</v>
       </c>
       <c r="E14" t="s">
         <v>30</v>
@@ -1630,85 +1661,89 @@
         <v>100</v>
       </c>
       <c r="N14" t="s">
-        <v>13</v>
+        <v>120</v>
       </c>
       <c r="O14" s="3">
-        <v>2298709129</v>
+        <v>677964975</v>
       </c>
       <c r="P14" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q14" s="3">
-        <v>1679195166.0999999</v>
-      </c>
-      <c r="R14"/>
+        <v>84</v>
+      </c>
+      <c r="Q14" s="3"/>
+      <c r="R14">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>93</v>
       </c>
       <c r="B15" s="7">
-        <v>15943589463</v>
+        <v>3426118654</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" t="s">
-        <v>3</v>
+        <v>93</v>
       </c>
       <c r="E15" t="s">
         <v>30</v>
       </c>
       <c r="F15" t="s">
-        <v>126</v>
+        <v>11</v>
       </c>
       <c r="G15" t="s">
         <v>114</v>
       </c>
       <c r="H15" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="I15" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="J15" t="s">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="K15" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="L15" t="s">
-        <v>131</v>
+        <v>4</v>
       </c>
       <c r="M15" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="N15" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="O15" s="3">
-        <v>2636263219</v>
+        <v>2298709129</v>
       </c>
       <c r="P15" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q15" s="3"/>
-      <c r="R15"/>
+        <v>26</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>1679195166.0999999</v>
+      </c>
+      <c r="R15">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>124</v>
-      </c>
-      <c r="B16" s="3">
-        <v>4469242245</v>
-      </c>
-      <c r="C16" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="B16" s="7">
+        <v>15943589463</v>
+      </c>
+      <c r="C16" s="7"/>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="E16" t="s">
         <v>30</v>
       </c>
       <c r="F16" t="s">
-        <v>30</v>
+        <v>126</v>
       </c>
       <c r="G16" t="s">
         <v>114</v>
@@ -1716,8 +1751,11 @@
       <c r="H16" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>69</v>
+      <c r="I16" t="s">
+        <v>126</v>
+      </c>
+      <c r="J16" t="s">
+        <v>126</v>
       </c>
       <c r="K16" t="s">
         <v>130</v>
@@ -1729,16 +1767,18 @@
         <v>130</v>
       </c>
       <c r="N16" t="s">
-        <v>121</v>
-      </c>
-      <c r="O16" s="4">
-        <v>2440888026</v>
-      </c>
-      <c r="P16" s="5" t="s">
-        <v>26</v>
+        <v>120</v>
+      </c>
+      <c r="O16" s="3">
+        <v>2636263219</v>
+      </c>
+      <c r="P16" t="s">
+        <v>132</v>
       </c>
       <c r="Q16" s="3"/>
-      <c r="R16"/>
+      <c r="R16">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
@@ -1764,7 +1804,7 @@
         <v>30</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="K17" t="s">
         <v>130</v>
@@ -1779,22 +1819,24 @@
         <v>121</v>
       </c>
       <c r="O17" s="4">
-        <v>2028354219</v>
+        <v>2440888026</v>
       </c>
       <c r="P17" s="5" t="s">
         <v>26</v>
       </c>
       <c r="Q17" s="3"/>
-      <c r="R17"/>
+      <c r="R17">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>125</v>
-      </c>
-      <c r="B18" s="7">
-        <v>2778017202</v>
-      </c>
-      <c r="C18" s="7"/>
+        <v>124</v>
+      </c>
+      <c r="B18" s="3">
+        <v>4469242245</v>
+      </c>
+      <c r="C18" s="3"/>
       <c r="D18" t="s">
         <v>29</v>
       </c>
@@ -1802,7 +1844,7 @@
         <v>30</v>
       </c>
       <c r="F18" t="s">
-        <v>126</v>
+        <v>30</v>
       </c>
       <c r="G18" t="s">
         <v>114</v>
@@ -1810,11 +1852,8 @@
       <c r="H18" t="s">
         <v>30</v>
       </c>
-      <c r="I18" t="s">
-        <v>126</v>
-      </c>
-      <c r="J18" t="s">
-        <v>126</v>
+      <c r="I18" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="K18" t="s">
         <v>130</v>
@@ -1829,127 +1868,133 @@
         <v>121</v>
       </c>
       <c r="O18" s="4">
-        <v>2290000000</v>
+        <v>2028354219</v>
+      </c>
+      <c r="P18" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="Q18" s="3"/>
-      <c r="R18"/>
+      <c r="R18">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>125</v>
       </c>
       <c r="B19" s="7">
-        <v>15943589463</v>
+        <v>2778017202</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
         <v>30</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>126</v>
       </c>
       <c r="G19" t="s">
         <v>114</v>
       </c>
       <c r="H19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I19" t="s">
-        <v>29</v>
+        <v>126</v>
       </c>
       <c r="J19" t="s">
-        <v>29</v>
+        <v>126</v>
       </c>
       <c r="K19" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="L19" t="s">
-        <v>29</v>
+        <v>131</v>
       </c>
       <c r="M19" t="s">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="N19" t="s">
-        <v>120</v>
-      </c>
-      <c r="O19" s="3">
-        <v>4984990736</v>
-      </c>
-      <c r="P19" t="s">
-        <v>85</v>
+        <v>121</v>
+      </c>
+      <c r="O19" s="4">
+        <v>2290000000</v>
       </c>
       <c r="Q19" s="3"/>
-      <c r="R19"/>
+      <c r="R19">
+        <v>4</v>
+      </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B20" s="7">
-        <v>24386112042.25</v>
+        <v>15943589463</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20" t="s">
         <v>30</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I20" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="J20" t="s">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="K20" t="s">
         <v>123</v>
       </c>
       <c r="L20" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="M20" t="s">
         <v>100</v>
       </c>
       <c r="N20" t="s">
-        <v>13</v>
+        <v>120</v>
       </c>
       <c r="O20" s="3">
-        <v>8127000000</v>
+        <v>4984990736</v>
       </c>
       <c r="P20" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="Q20" s="3"/>
-      <c r="R20"/>
+      <c r="R20">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B21" s="7">
-        <v>15943589463</v>
+        <v>24386112042.25</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E21" t="s">
         <v>30</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G21" t="s">
         <v>116</v>
@@ -1973,66 +2018,70 @@
         <v>100</v>
       </c>
       <c r="N21" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="O21" s="3">
-        <v>3518945000</v>
+        <v>8127000000</v>
       </c>
       <c r="P21" t="s">
-        <v>24</v>
+        <v>119</v>
       </c>
       <c r="Q21" s="3"/>
-      <c r="R21"/>
+      <c r="R21">
+        <v>6</v>
+      </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B22" s="7">
-        <v>24386112042.25</v>
+        <v>15943589463</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>113</v>
+        <v>30</v>
       </c>
       <c r="F22" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="G22" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I22" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="K22" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="L22" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="M22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N22" t="s">
-        <v>13</v>
+        <v>120</v>
       </c>
       <c r="O22" s="3">
-        <v>1615071673</v>
+        <v>3518945000</v>
       </c>
       <c r="P22" t="s">
-        <v>134</v>
+        <v>24</v>
       </c>
       <c r="Q22" s="3"/>
-      <c r="R22"/>
+      <c r="R22">
+        <v>3</v>
+      </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
@@ -2079,6 +2128,9 @@
         <v>355482847</v>
       </c>
       <c r="Q23" s="3"/>
+      <c r="R23" s="3">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -2219,7 +2271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9BDA4FF-EE12-4797-A020-C5630B964763}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+    <sheetView zoomScale="77" zoomScaleNormal="93" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>

</xml_diff>